<commit_message>
[Track] test cases finished
</commit_message>
<xml_diff>
--- a/utilities/car-count-test-cases.xlsx
+++ b/utilities/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="151">
   <si>
     <t>description</t>
   </si>
@@ -471,6 +471,9 @@
   </si>
   <si>
     <t>assign if not occluded</t>
+  </si>
+  <si>
+    <t>no change within backlash</t>
   </si>
 </sst>
 </file>
@@ -859,10 +862,10 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1149,7 @@
       <c r="A20" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="5" t="s">
         <v>148</v>
       </c>
       <c r="C20" t="s">
@@ -1154,6 +1157,9 @@
       </c>
       <c r="D20" s="8" t="s">
         <v>147</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,7 +1217,7 @@
       <c r="A24" t="s">
         <v>87</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C24" t="s">

</xml_diff>

<commit_message>
[Scene] test cases till #del001
</commit_message>
<xml_diff>
--- a/utilities/car-count-test-cases.xlsx
+++ b/utilities/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
   <si>
     <t>description</t>
   </si>
@@ -416,9 +416,6 @@
     <t>occ002</t>
   </si>
   <si>
-    <t>occ004</t>
-  </si>
-  <si>
     <t>occ003</t>
   </si>
   <si>
@@ -428,9 +425,6 @@
     <t>distance of opposite track entries</t>
   </si>
   <si>
-    <t>checkOcclusion</t>
-  </si>
-  <si>
     <t>steps in occusion</t>
   </si>
   <si>
@@ -452,9 +446,6 @@
     <t>del002</t>
   </si>
   <si>
-    <t>deleteReversinTracks</t>
-  </si>
-  <si>
     <t>same direction and intersection</t>
   </si>
   <si>
@@ -474,6 +465,16 @@
   </si>
   <si>
     <t>no change within backlash</t>
+  </si>
+  <si>
+    <t>getTrackID
+returnTrackID</t>
+  </si>
+  <si>
+    <t>keep track with longer history</t>
+  </si>
+  <si>
+    <t>deleteReversingTracks</t>
   </si>
 </sst>
 </file>
@@ -859,13 +860,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="H21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,16 +1151,16 @@
         <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D20" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1233,18 +1234,29 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="8"/>
     </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>88</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C28" t="s">
         <v>96</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>125</v>
@@ -1254,28 +1266,31 @@
       <c r="A29" t="s">
         <v>88</v>
       </c>
-      <c r="B29" t="s">
-        <v>138</v>
+      <c r="B29" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
-      <c r="B30" t="s">
-        <v>140</v>
+      <c r="B30" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,13 +1298,13 @@
         <v>88</v>
       </c>
       <c r="B31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="C31" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1320,7 +1335,7 @@
         <v>129</v>
       </c>
       <c r="D33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1328,54 +1343,57 @@
         <v>88</v>
       </c>
       <c r="B34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" t="s">
         <v>132</v>
       </c>
-      <c r="C34" t="s">
-        <v>133</v>
-      </c>
       <c r="D34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="B37" t="s">
         <v>109</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C37" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1383,13 +1401,10 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1397,45 +1412,34 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>13</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D49" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F49" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E53" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F53" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Scene] test cases till #occ002
</commit_message>
<xml_diff>
--- a/utilities/car-count-test-cases.xlsx
+++ b/utilities/car-count-test-cases.xlsx
@@ -863,10 +863,10 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="H21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1297,7 @@
       <c r="A31" t="s">
         <v>88</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>140</v>
       </c>
       <c r="C31" t="s">
@@ -1311,7 +1311,7 @@
       <c r="A32" t="s">
         <v>88</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C32" t="s">
@@ -1328,7 +1328,7 @@
       <c r="A33" t="s">
         <v>88</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C33" t="s">

</xml_diff>

<commit_message>
[Scene] test cases till #occ004
</commit_message>
<xml_diff>
--- a/utilities/car-count-test-cases.xlsx
+++ b/utilities/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="155">
   <si>
     <t>description</t>
   </si>
@@ -475,6 +475,18 @@
   </si>
   <si>
     <t>deleteReversingTracks</t>
+  </si>
+  <si>
+    <t>occ004</t>
+  </si>
+  <si>
+    <t>checkOcclusion</t>
+  </si>
+  <si>
+    <t>return occlusion area</t>
+  </si>
+  <si>
+    <t>execute only once</t>
   </si>
 </sst>
 </file>
@@ -863,10 +875,10 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,7 +1354,7 @@
       <c r="A34" t="s">
         <v>88</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>131</v>
       </c>
       <c r="C34" t="s">
@@ -1352,23 +1364,35 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>88</v>
       </c>
-      <c r="B35" t="s">
-        <v>135</v>
+      <c r="B35" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="D35" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>